<commit_message>
downloading the excel sheet only after choosing the directory path
</commit_message>
<xml_diff>
--- a/day2/users.xlsx
+++ b/day2/users.xlsx
@@ -13,25 +13,25 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>role</t>
-  </si>
-  <si>
-    <t>address</t>
-  </si>
-  <si>
-    <t>company</t>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Company</t>
   </si>
   <si>
     <t>abhi</t>
@@ -505,7 +505,9 @@
   <dimension ref="A1:G7"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="7" width="10" customWidth="1"/>
+    <col min="1" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="50" customWidth="1"/>
+    <col min="7" max="7" width="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>